<commit_message>
added export csv button
</commit_message>
<xml_diff>
--- a/test_data/FlowChart.xlsx
+++ b/test_data/FlowChart.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sakshi Narkhede\Downloads\Agent AI Prac\CSVCompareApp\test_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sakshi Narkhede\Downloads\dummy datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F91AE9AB-A038-4B0B-B52F-2539150A50E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED0DCE5F-B3A9-441E-ACA8-D0CBA7F1875C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{87707FA2-5A99-402B-AE24-C545E5CDE409}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="86">
   <si>
     <t>CHANNEL</t>
   </si>
@@ -761,9 +761,16 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1139,10 +1146,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F634F87A-298C-4C0A-8B82-5F80FB59D503}">
-  <dimension ref="A1:U14"/>
+  <dimension ref="A1:AD14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1150,73 +1157,82 @@
     <col min="1" max="1" width="23.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="U1" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
+      <c r="AA1" s="4"/>
+      <c r="AB1" s="4"/>
+      <c r="AC1" s="4"/>
+      <c r="AD1" s="4"/>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B2" t="s">
@@ -1280,10 +1296,8 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>21</v>
-      </c>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A3" s="2"/>
       <c r="B3" t="s">
         <v>22</v>
       </c>
@@ -1345,8 +1359,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B4" t="s">
@@ -1410,10 +1424,8 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>41</v>
-      </c>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A5" s="2"/>
       <c r="B5" t="s">
         <v>42</v>
       </c>
@@ -1475,10 +1487,8 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>41</v>
-      </c>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A6" s="2"/>
       <c r="B6" t="s">
         <v>58</v>
       </c>
@@ -1540,10 +1550,8 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>41</v>
-      </c>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A7" s="2"/>
       <c r="B7" t="s">
         <v>58</v>
       </c>
@@ -1605,10 +1613,8 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>41</v>
-      </c>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A8" s="2"/>
       <c r="B8" t="s">
         <v>59</v>
       </c>
@@ -1670,10 +1676,8 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>41</v>
-      </c>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A9" s="2"/>
       <c r="B9" t="s">
         <v>59</v>
       </c>
@@ -1735,8 +1739,8 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
         <v>60</v>
       </c>
       <c r="B10" t="s">
@@ -1800,10 +1804,8 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>60</v>
-      </c>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A11" s="3"/>
       <c r="B11" t="s">
         <v>61</v>
       </c>
@@ -1865,10 +1867,8 @@
         <v>40000</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>60</v>
-      </c>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A12" s="3"/>
       <c r="B12" t="s">
         <v>61</v>
       </c>
@@ -1930,10 +1930,8 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>60</v>
-      </c>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A13" s="3"/>
       <c r="B13" t="s">
         <v>81</v>
       </c>
@@ -1995,10 +1993,8 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>60</v>
-      </c>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A14" s="3"/>
       <c r="B14" t="s">
         <v>81</v>
       </c>
@@ -2061,6 +2057,11 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="A10:A14"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>